<commit_message>
Installer - Fix leap second bug that resulted in 32bit systems having a correct value of 37 leap seconds while 64bit systems had an incorrect value of 36 seconds.
</commit_message>
<xml_diff>
--- a/NOVAS/DeltaT Predictions/DeltaT Analysis 29th December 2016.xlsx
+++ b/NOVAS/DeltaT Predictions/DeltaT Analysis 29th December 2016.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ASCOM\NOVAS\DeltaT Predictions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ASCOM\NOVAS\DeltaT Predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,16 +15,16 @@
     <sheet name="DeltaT Analysis 24th October 15" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CoefC">'DeltaT Analysis 24th October 15'!$I$9</definedName>
-    <definedName name="CoefX">'DeltaT Analysis 24th October 15'!$I$8</definedName>
-    <definedName name="CoefX2">'DeltaT Analysis 24th October 15'!$I$7</definedName>
+    <definedName name="CoefC">'DeltaT Analysis 24th October 15'!$L$9</definedName>
+    <definedName name="CoefX">'DeltaT Analysis 24th October 15'!$L$8</definedName>
+    <definedName name="CoefX2">'DeltaT Analysis 24th October 15'!$L$7</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>TT-UT</t>
   </si>
@@ -82,6 +82,12 @@
   <si>
     <t>Long term</t>
   </si>
+  <si>
+    <t>Leap Secs</t>
+  </si>
+  <si>
+    <t>TT-UTC</t>
+  </si>
 </sst>
 </file>
 
@@ -90,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,8 +232,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +417,30 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -677,7 +713,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -723,6 +759,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="33" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="34" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="35" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="36" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="36" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1338,13 +1381,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>311726</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>128155</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>17318</xdr:rowOff>
@@ -1696,23 +1739,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K80"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="6"/>
-    <col min="7" max="7" width="4.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="6"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>2</v>
       </c>
@@ -1731,8 +1776,15 @@
       <c r="F1" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -1754,8 +1806,19 @@
         <f>D2-E2</f>
         <v>-2.2358187484883274E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="33">
+        <v>34</v>
+      </c>
+      <c r="H2" s="33">
+        <f>32.184+G2</f>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I2" s="33">
+        <f>H2-E2</f>
+        <v>-0.31345818748488341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -1777,9 +1840,20 @@
         <f t="shared" ref="F3:F22" si="2">D3-E3</f>
         <v>-3.6590546663290979E-2</v>
       </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="33">
+        <v>34</v>
+      </c>
+      <c r="H3" s="33">
+        <f t="shared" ref="H3:H66" si="3">32.184+G3</f>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I3" s="33">
+        <f t="shared" ref="I3:I66" si="4">H3-E3</f>
+        <v>-0.33549054666329425</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -1801,9 +1875,20 @@
         <f t="shared" si="2"/>
         <v>-3.6265327482809084E-2</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="33">
+        <v>34</v>
+      </c>
+      <c r="H4" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I4" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.35786532748281275</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -1825,9 +1910,20 @@
         <f t="shared" si="2"/>
         <v>-2.6282530001637383E-2</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="33">
+        <v>34</v>
+      </c>
+      <c r="H5" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I5" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.38058253000164655</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2011</v>
       </c>
@@ -1849,14 +1945,25 @@
         <f t="shared" si="2"/>
         <v>-1.7042154132482779E-2</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="33">
+        <v>34</v>
+      </c>
+      <c r="H6" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I6" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.40364215413248417</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2012</v>
       </c>
@@ -1878,14 +1985,25 @@
         <f t="shared" si="2"/>
         <v>-8.0441999917439944E-3</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="G7" s="33">
+        <v>34</v>
+      </c>
+      <c r="H7" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I7" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.42704419999174092</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="17">
+      <c r="L7" s="17">
         <v>2.465436E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2012</v>
       </c>
@@ -1907,14 +2025,25 @@
         <f t="shared" si="2"/>
         <v>-7.8866750665440577E-4</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" s="33">
+        <v>34</v>
+      </c>
+      <c r="H8" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I8" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.45078866750665725</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="18">
+      <c r="L8" s="18">
         <v>-98.926265560000004</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2012</v>
       </c>
@@ -1936,14 +2065,25 @@
         <f t="shared" si="2"/>
         <v>-1.9755566481336473E-3</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="G9" s="33">
+        <v>34</v>
+      </c>
+      <c r="H9" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I9" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.4748755566481293</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="19">
+      <c r="L9" s="19">
         <v>99301.857843079997</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -1965,8 +2105,19 @@
         <f t="shared" si="2"/>
         <v>9.1951324965293679E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="33">
+        <v>34</v>
+      </c>
+      <c r="H10" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I10" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.49930486750346859</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -1988,12 +2139,23 @@
         <f t="shared" si="2"/>
         <v>2.0823400014634785E-2</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="G11" s="33">
+        <v>34</v>
+      </c>
+      <c r="H11" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I11" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.5240765999853636</v>
+      </c>
+      <c r="K11" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="30"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L11" s="30"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -2015,16 +2177,27 @@
         <f t="shared" si="2"/>
         <v>2.4709245847986949E-2</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21" t="s">
+      <c r="G12" s="33">
+        <v>34</v>
+      </c>
+      <c r="H12" s="33">
+        <f t="shared" si="3"/>
+        <v>66.183999999999997</v>
+      </c>
+      <c r="I12" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.54919075415202201</v>
+      </c>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="16">
+      <c r="L12" s="16">
         <f>_xlfn.STDEV.P(F2:F61)</f>
         <v>2.7067256878862522E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2012</v>
       </c>
@@ -2046,16 +2219,27 @@
         <f t="shared" si="2"/>
         <v>1.2152669996552845E-2</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="22" t="s">
+      <c r="G13" s="34">
+        <v>35</v>
+      </c>
+      <c r="H13" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I13" s="34">
+        <f t="shared" si="4"/>
+        <v>0.42535266999655619</v>
+      </c>
+      <c r="J13" s="20"/>
+      <c r="K13" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="24">
+      <c r="L13" s="24">
         <f>_xlfn.STDEV.P(F62:F73)</f>
         <v>5.2965148877899479E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -2077,16 +2261,27 @@
         <f t="shared" si="2"/>
         <v>-1.0446327481417939E-2</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="23" t="s">
+      <c r="G14" s="34">
+        <v>35</v>
+      </c>
+      <c r="H14" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I14" s="34">
+        <f t="shared" si="4"/>
+        <v>0.39955367251857865</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="25">
+      <c r="L14" s="25">
         <f>_xlfn.STDEV.P(F74:F80)</f>
         <v>0.26105664776816889</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2012</v>
       </c>
@@ -2108,8 +2303,19 @@
         <f t="shared" si="2"/>
         <v>-2.5987746658714173E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="34">
+        <v>35</v>
+      </c>
+      <c r="H15" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I15" s="34">
+        <f t="shared" si="4"/>
+        <v>0.3734122533412858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
@@ -2131,8 +2337,19 @@
         <f t="shared" si="2"/>
         <v>-2.6771587477114167E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="34">
+        <v>35</v>
+      </c>
+      <c r="H16" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I16" s="34">
+        <f t="shared" si="4"/>
+        <v>0.34692841252288531</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2012</v>
       </c>
@@ -2154,9 +2371,20 @@
         <f t="shared" si="2"/>
         <v>-2.3897849994824583E-2</v>
       </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="34">
+        <v>35</v>
+      </c>
+      <c r="H17" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I17" s="34">
+        <f t="shared" si="4"/>
+        <v>0.32010215000516951</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2012</v>
       </c>
@@ -2178,9 +2406,20 @@
         <f t="shared" si="2"/>
         <v>-1.3166534168206567E-2</v>
       </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="34">
+        <v>35</v>
+      </c>
+      <c r="H18" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I18" s="34">
+        <f t="shared" si="4"/>
+        <v>0.29293346583179414</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2013</v>
       </c>
@@ -2202,9 +2441,20 @@
         <f t="shared" si="2"/>
         <v>-1.1677639982693222E-2</v>
       </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="34">
+        <v>35</v>
+      </c>
+      <c r="H19" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I19" s="34">
+        <f t="shared" si="4"/>
+        <v>0.26542236001731112</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -2226,9 +2476,20 @@
         <f t="shared" si="2"/>
         <v>-2.1311674964863414E-3</v>
       </c>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="34">
+        <v>35</v>
+      </c>
+      <c r="H20" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I20" s="34">
+        <f t="shared" si="4"/>
+        <v>0.23756883250351279</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2013</v>
       </c>
@@ -2250,9 +2511,20 @@
         <f t="shared" si="2"/>
         <v>1.6728833631560747E-3</v>
       </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="34">
+        <v>35</v>
+      </c>
+      <c r="H21" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I21" s="34">
+        <f t="shared" si="4"/>
+        <v>0.20937288336315873</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2013</v>
       </c>
@@ -2274,9 +2546,20 @@
         <f t="shared" si="2"/>
         <v>2.2634512508943772E-2</v>
       </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="34">
+        <v>35</v>
+      </c>
+      <c r="H22" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I22" s="34">
+        <f t="shared" si="4"/>
+        <v>0.18083451250893745</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2013</v>
       </c>
@@ -2291,16 +2574,27 @@
         <v>67.071600000000004</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" ref="E23:E31" si="3">(CoefX2*C23*C23)+(CoefX*C23) +CoefC</f>
+        <f t="shared" ref="E23:E31" si="5">(CoefX2*C23*C23)+(CoefX*C23) +CoefC</f>
         <v>67.032046279971837</v>
       </c>
       <c r="F23" s="9">
-        <f t="shared" ref="F23:F31" si="4">D23-E23</f>
+        <f t="shared" ref="F23:F31" si="6">D23-E23</f>
         <v>3.9553720028166595E-2</v>
       </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="34">
+        <v>35</v>
+      </c>
+      <c r="H23" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I23" s="34">
+        <f t="shared" si="4"/>
+        <v>0.15195372002816043</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2013</v>
       </c>
@@ -2315,16 +2609,27 @@
         <v>67.11</v>
       </c>
       <c r="E24" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.061269494151929</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.8730505848070038E-2</v>
       </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="34">
+        <v>35</v>
+      </c>
+      <c r="H24" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I24" s="34">
+        <f t="shared" si="4"/>
+        <v>0.12273050584806811</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -2339,16 +2644,27 @@
         <v>67.126599999999996</v>
       </c>
       <c r="E25" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.090835130002233</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.5764869997763071E-2</v>
       </c>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="34">
+        <v>35</v>
+      </c>
+      <c r="H25" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I25" s="34">
+        <f t="shared" si="4"/>
+        <v>9.3164869997764299E-2</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2013</v>
       </c>
@@ -2363,16 +2679,27 @@
         <v>67.133099999999999</v>
       </c>
       <c r="E26" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.120743187479093</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2356812520906146E-2</v>
       </c>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="34">
+        <v>35</v>
+      </c>
+      <c r="H26" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I26" s="34">
+        <f t="shared" si="4"/>
+        <v>6.3256812520904759E-2</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2013</v>
       </c>
@@ -2387,16 +2714,27 @@
         <v>67.145799999999994</v>
       </c>
       <c r="E27" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.150993666655268</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-5.1936666552734323E-3</v>
       </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="34">
+        <v>35</v>
+      </c>
+      <c r="H27" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I27" s="34">
+        <f t="shared" si="4"/>
+        <v>3.300633334472991E-2</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2013</v>
       </c>
@@ -2411,16 +2749,27 @@
         <v>67.171700000000001</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.18158656747255</v>
       </c>
       <c r="F28" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-9.8865674725487906E-3</v>
       </c>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="34">
+        <v>35</v>
+      </c>
+      <c r="H28" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I28" s="34">
+        <f t="shared" si="4"/>
+        <v>2.4134325274474122E-3</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2013</v>
       </c>
@@ -2435,16 +2784,27 @@
         <v>67.209100000000007</v>
       </c>
       <c r="E29" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.212521889989148</v>
       </c>
       <c r="F29" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-3.4218899891413912E-3</v>
       </c>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="34">
+        <v>35</v>
+      </c>
+      <c r="H29" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I29" s="34">
+        <f t="shared" si="4"/>
+        <v>-2.8521889989150395E-2</v>
+      </c>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2013</v>
       </c>
@@ -2459,16 +2819,27 @@
         <v>67.245999999999995</v>
       </c>
       <c r="E30" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.243799634161405</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.2003658385898461E-3</v>
       </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="34">
+        <v>35</v>
+      </c>
+      <c r="H30" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I30" s="34">
+        <f t="shared" si="4"/>
+        <v>-5.9799634161407766E-2</v>
+      </c>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2014</v>
       </c>
@@ -2483,16 +2854,27 @@
         <v>67.281000000000006</v>
       </c>
       <c r="E31" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>67.275419799989322</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.5802000106837113E-3</v>
       </c>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="34">
+        <v>35</v>
+      </c>
+      <c r="H31" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I31" s="34">
+        <f t="shared" si="4"/>
+        <v>-9.1419799989324702E-2</v>
+      </c>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2014</v>
       </c>
@@ -2507,16 +2889,27 @@
         <v>67.313599999999994</v>
       </c>
       <c r="E32" s="7">
-        <f t="shared" ref="E32" si="5">(CoefX2*C32*C32)+(CoefX*C32) +CoefC</f>
+        <f t="shared" ref="E32" si="7">(CoefX2*C32*C32)+(CoefX*C32) +CoefC</f>
         <v>67.307382387487451</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" ref="F32" si="6">D32-E32</f>
+        <f t="shared" ref="F32" si="8">D32-E32</f>
         <v>6.2176125125432691E-3</v>
       </c>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G32" s="34">
+        <v>35</v>
+      </c>
+      <c r="H32" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I32" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.12338238748745312</v>
+      </c>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2014</v>
       </c>
@@ -2531,16 +2924,27 @@
         <v>67.345699999999994</v>
       </c>
       <c r="E33" s="7">
-        <f t="shared" ref="E33:E52" si="7">(CoefX2*C33*C33)+(CoefX*C33) +CoefC</f>
+        <f t="shared" ref="E33:E52" si="9">(CoefX2*C33*C33)+(CoefX*C33) +CoefC</f>
         <v>67.339687396641239</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" ref="F33:F52" si="8">D33-E33</f>
+        <f t="shared" ref="F33:F52" si="10">D33-E33</f>
         <v>6.0126033587550864E-3</v>
       </c>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G33" s="34">
+        <v>35</v>
+      </c>
+      <c r="H33" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I33" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.15568739664124109</v>
+      </c>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2014</v>
       </c>
@@ -2548,23 +2952,34 @@
         <v>4</v>
       </c>
       <c r="C34" s="9">
-        <f t="shared" ref="C34:C61" si="9">A34+(B34-1)/12</f>
+        <f t="shared" ref="C34:C61" si="11">A34+(B34-1)/12</f>
         <v>2014.25</v>
       </c>
       <c r="D34" s="7">
         <v>67.388999999999996</v>
       </c>
       <c r="E34" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.372334827494342</v>
       </c>
       <c r="F34" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.6665172505653914E-2</v>
       </c>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G34" s="34">
+        <v>35</v>
+      </c>
+      <c r="H34" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I34" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.18833482749434438</v>
+      </c>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2014</v>
       </c>
@@ -2572,23 +2987,34 @@
         <v>5</v>
       </c>
       <c r="C35" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.3333333333333</v>
       </c>
       <c r="D35" s="7">
         <v>67.431799999999996</v>
       </c>
       <c r="E35" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.405324680003105</v>
       </c>
       <c r="F35" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.6475319996890789E-2</v>
       </c>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="34">
+        <v>35</v>
+      </c>
+      <c r="H35" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I35" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.22132468000310723</v>
+      </c>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2014</v>
       </c>
@@ -2596,23 +3022,34 @@
         <v>6</v>
       </c>
       <c r="C36" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.4166666666667</v>
       </c>
       <c r="D36" s="7">
         <v>67.4666</v>
       </c>
       <c r="E36" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.438656954138423</v>
       </c>
       <c r="F36" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.7943045861576365E-2</v>
       </c>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G36" s="34">
+        <v>35</v>
+      </c>
+      <c r="H36" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I36" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.25465695413842582</v>
+      </c>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2014</v>
       </c>
@@ -2620,23 +3057,34 @@
         <v>7</v>
       </c>
       <c r="C37" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.5</v>
       </c>
       <c r="D37" s="7">
         <v>67.485799999999998</v>
       </c>
       <c r="E37" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.472331650002161</v>
       </c>
       <c r="F37" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.3468349997836526E-2</v>
       </c>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G37" s="34">
+        <v>35</v>
+      </c>
+      <c r="H37" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I37" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.28833165000216354</v>
+      </c>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2014</v>
       </c>
@@ -2644,25 +3092,36 @@
         <v>8</v>
       </c>
       <c r="C38" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.5833333333333</v>
       </c>
       <c r="D38" s="7">
         <v>67.498900000000006</v>
       </c>
       <c r="E38" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.506348767477903</v>
       </c>
       <c r="F38" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-7.4487674778964674E-3</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="G38" s="34">
+        <v>35</v>
+      </c>
+      <c r="H38" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I38" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.32234876747790508</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2014</v>
       </c>
@@ -2670,23 +3129,34 @@
         <v>9</v>
       </c>
       <c r="C39" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.6666666666667</v>
       </c>
       <c r="D39" s="7">
         <v>67.511099999999999</v>
       </c>
       <c r="E39" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.540708306652959</v>
       </c>
       <c r="F39" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.9608306652960437E-2</v>
       </c>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G39" s="34">
+        <v>35</v>
+      </c>
+      <c r="H39" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I39" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.35670830665296194</v>
+      </c>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2014</v>
       </c>
@@ -2694,28 +3164,39 @@
         <v>10</v>
       </c>
       <c r="C40" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.75</v>
       </c>
       <c r="D40" s="7">
         <v>67.535300000000007</v>
       </c>
       <c r="E40" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.575410267498228</v>
       </c>
       <c r="F40" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.0110267498221219E-2</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="G40" s="34">
+        <v>35</v>
+      </c>
+      <c r="H40" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I40" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.39141026749823027</v>
+      </c>
+      <c r="K40" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2014</v>
       </c>
@@ -2723,28 +3204,39 @@
         <v>11</v>
       </c>
       <c r="C41" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.8333333333333</v>
       </c>
       <c r="D41" s="7">
         <v>67.571100000000001</v>
       </c>
       <c r="E41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.610454649984604</v>
       </c>
       <c r="F41" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.9354649984602474E-2</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="G41" s="34">
+        <v>35</v>
+      </c>
+      <c r="H41" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I41" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.42645464998460625</v>
+      </c>
+      <c r="K41" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2014</v>
       </c>
@@ -2752,28 +3244,39 @@
         <v>12</v>
       </c>
       <c r="C42" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2014.9166666666667</v>
       </c>
       <c r="D42" s="7">
         <v>67.606999999999999</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.645841454155743</v>
       </c>
       <c r="F42" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.8841454155743804E-2</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="G42" s="34">
+        <v>35</v>
+      </c>
+      <c r="H42" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I42" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.46184145415574562</v>
+      </c>
+      <c r="K42" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2015</v>
       </c>
@@ -2781,23 +3284,34 @@
         <v>1</v>
       </c>
       <c r="C43" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D43" s="7">
         <v>67.643900000000002</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.681570679982542</v>
       </c>
       <c r="F43" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.7670679982539923E-2</v>
       </c>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G43" s="34">
+        <v>35</v>
+      </c>
+      <c r="H43" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I43" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.49757067998254456</v>
+      </c>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2015</v>
       </c>
@@ -2805,23 +3319,34 @@
         <v>2</v>
       </c>
       <c r="C44" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.0833333333333</v>
       </c>
       <c r="D44" s="7">
         <v>67.676500000000004</v>
       </c>
       <c r="E44" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.717642327494104</v>
       </c>
       <c r="F44" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.1142327494100073E-2</v>
       </c>
-      <c r="G44" s="5"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G44" s="34">
+        <v>35</v>
+      </c>
+      <c r="H44" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I44" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.53364232749410689</v>
+      </c>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2015</v>
       </c>
@@ -2829,23 +3354,34 @@
         <v>3</v>
       </c>
       <c r="C45" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.1666666666667</v>
       </c>
       <c r="D45" s="7">
         <v>67.711699999999993</v>
       </c>
       <c r="E45" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.754056396661326</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.2356396661332951E-2</v>
       </c>
-      <c r="G45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G45" s="34">
+        <v>35</v>
+      </c>
+      <c r="H45" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I45" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.57005639666132879</v>
+      </c>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2015</v>
       </c>
@@ -2853,23 +3389,34 @@
         <v>4</v>
       </c>
       <c r="C46" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.25</v>
       </c>
       <c r="D46" s="7">
         <v>67.759100000000004</v>
       </c>
       <c r="E46" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.790812887484208</v>
       </c>
       <c r="F46" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.1712887484204089E-2</v>
       </c>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G46" s="34">
+        <v>35</v>
+      </c>
+      <c r="H46" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I46" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.60681288748421025</v>
+      </c>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -2877,23 +3424,34 @@
         <v>5</v>
       </c>
       <c r="C47" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.3333333333333</v>
       </c>
       <c r="D47" s="7">
         <v>67.801100000000005</v>
       </c>
       <c r="E47" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.827911799991853</v>
       </c>
       <c r="F47" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.6811799991847352E-2</v>
       </c>
-      <c r="G47" s="5"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G47" s="34">
+        <v>35</v>
+      </c>
+      <c r="H47" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I47" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.6439117999918551</v>
+      </c>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2015</v>
       </c>
@@ -2901,23 +3459,34 @@
         <v>6</v>
       </c>
       <c r="C48" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.4166666666667</v>
       </c>
       <c r="D48" s="7">
         <v>67.840199999999996</v>
       </c>
       <c r="E48" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.865353134140605</v>
       </c>
       <c r="F48" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.5153134140609268E-2</v>
       </c>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="34">
+        <v>35</v>
+      </c>
+      <c r="H48" s="34">
+        <f t="shared" si="3"/>
+        <v>67.183999999999997</v>
+      </c>
+      <c r="I48" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.68135313414060761</v>
+      </c>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2015</v>
       </c>
@@ -2925,23 +3494,34 @@
         <v>7</v>
       </c>
       <c r="C49" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.5</v>
       </c>
       <c r="D49" s="7">
         <v>67.860600000000005</v>
       </c>
       <c r="E49" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.903136889988673</v>
       </c>
       <c r="F49" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.2536889988667781E-2</v>
       </c>
-      <c r="G49" s="5"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="35">
+        <v>36</v>
+      </c>
+      <c r="H49" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I49" s="35">
+        <f t="shared" si="4"/>
+        <v>0.28086311001132458</v>
+      </c>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2015</v>
       </c>
@@ -2949,23 +3529,34 @@
         <v>8</v>
       </c>
       <c r="C50" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.5833333333333</v>
       </c>
       <c r="D50" s="7">
         <v>67.882199999999997</v>
       </c>
       <c r="E50" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.941263067477848</v>
       </c>
       <c r="F50" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-5.906306747785095E-2</v>
       </c>
-      <c r="G50" s="5"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="35">
+        <v>36</v>
+      </c>
+      <c r="H50" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I50" s="35">
+        <f t="shared" si="4"/>
+        <v>0.24273693252214912</v>
+      </c>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2015</v>
       </c>
@@ -2973,23 +3564,34 @@
         <v>9</v>
       </c>
       <c r="C51" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.6666666666667</v>
       </c>
       <c r="D51" s="7">
         <v>67.912000000000006</v>
       </c>
       <c r="E51" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67.979731666651787</v>
       </c>
       <c r="F51" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-6.7731666651781097E-2</v>
       </c>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="35">
+        <v>36</v>
+      </c>
+      <c r="H51" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I51" s="35">
+        <f t="shared" si="4"/>
+        <v>0.20426833334821026</v>
+      </c>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2015</v>
       </c>
@@ -2997,23 +3599,34 @@
         <v>10</v>
       </c>
       <c r="C52" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.75</v>
       </c>
       <c r="D52" s="7">
         <v>67.954700000000003</v>
       </c>
       <c r="E52" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>68.018542687495938</v>
       </c>
       <c r="F52" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-6.3842687495935024E-2</v>
       </c>
-      <c r="G52" s="5"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="35">
+        <v>36</v>
+      </c>
+      <c r="H52" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I52" s="35">
+        <f t="shared" si="4"/>
+        <v>0.16545731250405993</v>
+      </c>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2015</v>
       </c>
@@ -3021,22 +3634,33 @@
         <v>11</v>
       </c>
       <c r="C53" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.8333333333333</v>
       </c>
       <c r="D53" s="7">
         <v>68.005499999999998</v>
       </c>
       <c r="E53" s="7">
-        <f t="shared" ref="E53:E80" si="10">(CoefX2*C53*C53)+(CoefX*C53) +CoefC</f>
+        <f t="shared" ref="E53:E80" si="12">(CoefX2*C53*C53)+(CoefX*C53) +CoefC</f>
         <v>68.057696129981196</v>
       </c>
       <c r="F53" s="9">
-        <f t="shared" ref="F53:F80" si="11">D53-E53</f>
+        <f t="shared" ref="F53:F80" si="13">D53-E53</f>
         <v>-5.2196129981197714E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="35">
+        <v>36</v>
+      </c>
+      <c r="H53" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I53" s="35">
+        <f t="shared" si="4"/>
+        <v>0.12630387001880194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2015</v>
       </c>
@@ -3044,23 +3668,34 @@
         <v>12</v>
       </c>
       <c r="C54" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2015.9166666666667</v>
       </c>
       <c r="D54" s="7">
         <v>68.051400000000001</v>
       </c>
       <c r="E54" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.097191994165769</v>
       </c>
       <c r="F54" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-4.5791994165767846E-2</v>
       </c>
-      <c r="G54" s="5"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="35">
+        <v>36</v>
+      </c>
+      <c r="H54" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I54" s="35">
+        <f t="shared" si="4"/>
+        <v>8.6808005834228652E-2</v>
+      </c>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2016</v>
       </c>
@@ -3068,23 +3703,34 @@
         <v>1</v>
       </c>
       <c r="C55" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2016</v>
       </c>
       <c r="D55" s="7">
         <v>68.102400000000003</v>
       </c>
       <c r="E55" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.137030279976898</v>
       </c>
       <c r="F55" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-3.463027997689494E-2</v>
       </c>
-      <c r="G55" s="5"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="35">
+        <v>36</v>
+      </c>
+      <c r="H55" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I55" s="35">
+        <f t="shared" si="4"/>
+        <v>4.6969720023099626E-2</v>
+      </c>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2016</v>
       </c>
@@ -3092,23 +3738,34 @@
         <v>2</v>
       </c>
       <c r="C56" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2016.0833333333333</v>
       </c>
       <c r="D56" s="7">
         <v>68.157700000000006</v>
       </c>
       <c r="E56" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.177210987487342</v>
       </c>
       <c r="F56" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1.9510987487336706E-2</v>
       </c>
-      <c r="G56" s="5"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="35">
+        <v>36</v>
+      </c>
+      <c r="H56" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I56" s="35">
+        <f t="shared" si="4"/>
+        <v>6.7890125126552903E-3</v>
+      </c>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2016</v>
       </c>
@@ -3116,23 +3773,34 @@
         <v>3</v>
       </c>
       <c r="C57" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2016.1666666666667</v>
       </c>
       <c r="D57" s="7">
         <v>68.204400000000007</v>
       </c>
       <c r="E57" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.217734116667998</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1.3334116667991225E-2</v>
       </c>
-      <c r="G57" s="5"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="35">
+        <v>36</v>
+      </c>
+      <c r="H57" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I57" s="35">
+        <f t="shared" si="4"/>
+        <v>-3.3734116668000524E-2</v>
+      </c>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2016</v>
       </c>
@@ -3140,23 +3808,34 @@
         <v>4</v>
       </c>
       <c r="C58" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2016.25</v>
       </c>
       <c r="D58" s="7">
         <v>68.266499999999994</v>
       </c>
       <c r="E58" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.258599667489761</v>
       </c>
       <c r="F58" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.9003325102320332E-3</v>
       </c>
-      <c r="G58" s="5"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="35">
+        <v>36</v>
+      </c>
+      <c r="H58" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I58" s="35">
+        <f t="shared" si="4"/>
+        <v>-7.4599667489763988E-2</v>
+      </c>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2016</v>
       </c>
@@ -3164,23 +3843,34 @@
         <v>5</v>
       </c>
       <c r="C59" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2016.3333333333333</v>
       </c>
       <c r="D59" s="7">
         <v>68.318799999999996</v>
       </c>
       <c r="E59" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.299807639996288</v>
       </c>
       <c r="F59" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.8992360003707631E-2</v>
       </c>
-      <c r="G59" s="5"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="35">
+        <v>36</v>
+      </c>
+      <c r="H59" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I59" s="35">
+        <f t="shared" si="4"/>
+        <v>-0.11580763999629085</v>
+      </c>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2016</v>
       </c>
@@ -3188,23 +3878,34 @@
         <v>6</v>
       </c>
       <c r="C60" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2016.4166666666667</v>
       </c>
       <c r="D60" s="7">
         <v>68.3703</v>
       </c>
       <c r="E60" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.341358034143923</v>
       </c>
       <c r="F60" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.8941965856077445E-2</v>
       </c>
-      <c r="G60" s="5"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G60" s="35">
+        <v>36</v>
+      </c>
+      <c r="H60" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I60" s="35">
+        <f t="shared" si="4"/>
+        <v>-0.15735803414392535</v>
+      </c>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2016</v>
       </c>
@@ -3212,23 +3913,34 @@
         <v>7</v>
       </c>
       <c r="C61" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2016.5</v>
       </c>
       <c r="D61" s="7">
         <v>68.3964</v>
       </c>
       <c r="E61" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.383250849990873</v>
       </c>
       <c r="F61" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.3149150009127197E-2</v>
       </c>
-      <c r="G61" s="5"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G61" s="35">
+        <v>36</v>
+      </c>
+      <c r="H61" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I61" s="35">
+        <f t="shared" si="4"/>
+        <v>-0.19925084999087517</v>
+      </c>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C62" s="15">
         <v>2016.75</v>
       </c>
@@ -3236,16 +3948,27 @@
         <v>68.510000000000005</v>
       </c>
       <c r="E62" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.510983827494783</v>
       </c>
       <c r="F62" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-9.8382749477821108E-4</v>
       </c>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G62" s="35">
+        <v>36</v>
+      </c>
+      <c r="H62" s="35">
+        <f t="shared" si="3"/>
+        <v>68.183999999999997</v>
+      </c>
+      <c r="I62" s="35">
+        <f t="shared" si="4"/>
+        <v>-0.32698382749478583</v>
+      </c>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C63" s="15">
         <v>2017</v>
       </c>
@@ -3253,16 +3976,27 @@
         <v>68.66</v>
       </c>
       <c r="E63" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.641798600001493</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.8201399998503121E-2</v>
       </c>
-      <c r="G63" s="5"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G63" s="36">
+        <v>37</v>
+      </c>
+      <c r="H63" s="37">
+        <f t="shared" si="3"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I63" s="37">
+        <f t="shared" si="4"/>
+        <v>0.54220139999850403</v>
+      </c>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C64" s="15">
         <v>2017.25</v>
       </c>
@@ -3270,15 +4004,26 @@
         <v>68.8</v>
       </c>
       <c r="E64" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.775695167481899</v>
       </c>
       <c r="F64" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.4304832518097896E-2</v>
       </c>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G64" s="36">
+        <v>37</v>
+      </c>
+      <c r="H64" s="37">
+        <f t="shared" si="3"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I64" s="37">
+        <f t="shared" si="4"/>
+        <v>0.40830483251809824</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C65" s="15">
         <v>2017.5</v>
       </c>
@@ -3286,16 +4031,27 @@
         <v>69</v>
       </c>
       <c r="E65" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68.912673529979656</v>
       </c>
       <c r="F65" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.732647002034355E-2</v>
       </c>
-      <c r="G65" s="5"/>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G65" s="36">
+        <v>37</v>
+      </c>
+      <c r="H65" s="37">
+        <f t="shared" si="3"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I65" s="37">
+        <f t="shared" si="4"/>
+        <v>0.27132647002034105</v>
+      </c>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C66" s="15">
         <v>2017.75</v>
       </c>
@@ -3303,16 +4059,27 @@
         <v>69.099999999999994</v>
       </c>
       <c r="E66" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69.052733687494765</v>
       </c>
       <c r="F66" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.726631250522928E-2</v>
       </c>
-      <c r="G66" s="5"/>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G66" s="36">
+        <v>37</v>
+      </c>
+      <c r="H66" s="37">
+        <f t="shared" si="3"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I66" s="37">
+        <f t="shared" si="4"/>
+        <v>0.13126631250523246</v>
+      </c>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C67" s="15">
         <v>2018</v>
       </c>
@@ -3320,16 +4087,27 @@
         <v>69.2</v>
       </c>
       <c r="E67" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69.195875639998121</v>
       </c>
       <c r="F67" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.1243600018816551E-3</v>
       </c>
-      <c r="G67" s="5"/>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G67" s="36">
+        <v>37</v>
+      </c>
+      <c r="H67" s="37">
+        <f t="shared" ref="H67:H73" si="14">32.184+G67</f>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I67" s="37">
+        <f t="shared" ref="I67:I73" si="15">H67-E67</f>
+        <v>-1.1875639998123688E-2</v>
+      </c>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C68" s="15">
         <v>2018.25</v>
       </c>
@@ -3337,16 +4115,27 @@
         <v>69.400000000000006</v>
       </c>
       <c r="E68" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69.342099387475173</v>
       </c>
       <c r="F68" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.7900612524832695E-2</v>
       </c>
-      <c r="G68" s="5"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="36">
+        <v>37</v>
+      </c>
+      <c r="H68" s="37">
+        <f t="shared" si="14"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I68" s="37">
+        <f t="shared" si="15"/>
+        <v>-0.15809938747517549</v>
+      </c>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C69" s="15">
         <v>2018.5</v>
       </c>
@@ -3354,16 +4143,27 @@
         <v>69.5</v>
       </c>
       <c r="E69" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69.491404929984128</v>
       </c>
       <c r="F69" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.5950700158718973E-3</v>
       </c>
-      <c r="G69" s="5"/>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G69" s="36">
+        <v>37</v>
+      </c>
+      <c r="H69" s="37">
+        <f t="shared" si="14"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I69" s="37">
+        <f t="shared" si="15"/>
+        <v>-0.3074049299841306</v>
+      </c>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" s="15">
         <v>2018.75</v>
       </c>
@@ -3371,16 +4171,27 @@
         <v>69.7</v>
       </c>
       <c r="E70" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69.643792267481331</v>
       </c>
       <c r="F70" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.620773251867206E-2</v>
       </c>
-      <c r="G70" s="5"/>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="36">
+        <v>37</v>
+      </c>
+      <c r="H70" s="37">
+        <f t="shared" si="14"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I70" s="37">
+        <f t="shared" si="15"/>
+        <v>-0.45979226748133328</v>
+      </c>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C71" s="15">
         <v>2019</v>
       </c>
@@ -3388,16 +4199,27 @@
         <v>69.8</v>
       </c>
       <c r="E71" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69.799261399995885</v>
       </c>
       <c r="F71" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.3860000411229976E-4</v>
       </c>
-      <c r="G71" s="5"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="36">
+        <v>37</v>
+      </c>
+      <c r="H71" s="37">
+        <f t="shared" si="14"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I71" s="37">
+        <f t="shared" si="15"/>
+        <v>-0.61526139999588736</v>
+      </c>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C72" s="15">
         <v>2019.25</v>
       </c>
@@ -3405,16 +4227,27 @@
         <v>69.900000000000006</v>
       </c>
       <c r="E72" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69.957812327498686</v>
       </c>
       <c r="F72" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-5.7812327498680816E-2</v>
       </c>
-      <c r="G72" s="5"/>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G72" s="36">
+        <v>37</v>
+      </c>
+      <c r="H72" s="37">
+        <f t="shared" si="14"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I72" s="37">
+        <f t="shared" si="15"/>
+        <v>-0.773812327498689</v>
+      </c>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C73" s="15">
         <v>2019.5</v>
       </c>
@@ -3422,16 +4255,27 @@
         <v>70</v>
       </c>
       <c r="E73" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70.119445049975184</v>
       </c>
       <c r="F73" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-0.11944504997518379</v>
       </c>
-      <c r="G73" s="5"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="36">
+        <v>37</v>
+      </c>
+      <c r="H73" s="37">
+        <f t="shared" si="14"/>
+        <v>69.183999999999997</v>
+      </c>
+      <c r="I73" s="37">
+        <f t="shared" si="15"/>
+        <v>-0.93544504997518629</v>
+      </c>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C74" s="12">
         <v>2019.75</v>
       </c>
@@ -3439,16 +4283,19 @@
         <v>70</v>
       </c>
       <c r="E74" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70.284159567483584</v>
       </c>
       <c r="F74" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-0.2841595674835844</v>
       </c>
-      <c r="G74" s="5"/>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G74" s="31"/>
+      <c r="H74" s="31"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C75" s="12">
         <v>2020</v>
       </c>
@@ -3456,16 +4303,19 @@
         <v>70</v>
       </c>
       <c r="E75" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70.451955879994784</v>
       </c>
       <c r="F75" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-0.45195587999478448</v>
       </c>
-      <c r="G75" s="5"/>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C76" s="12">
         <v>2020.25</v>
       </c>
@@ -3473,16 +4323,19 @@
         <v>70</v>
       </c>
       <c r="E76" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70.622833987494232</v>
       </c>
       <c r="F76" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-0.62283398749423213</v>
       </c>
-      <c r="G76" s="5"/>
-    </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G76" s="31"/>
+      <c r="H76" s="31"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C77" s="12">
         <v>2020.5</v>
       </c>
@@ -3490,15 +4343,18 @@
         <v>71</v>
       </c>
       <c r="E77" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70.796793889967375</v>
       </c>
       <c r="F77" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.20320611003262457</v>
       </c>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="31"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C78" s="12">
         <v>2020.75</v>
       </c>
@@ -3506,15 +4362,18 @@
         <v>71</v>
       </c>
       <c r="E78" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70.973835587472422</v>
       </c>
       <c r="F78" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.6164412527577952E-2</v>
       </c>
-    </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G78" s="31"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="31"/>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C79" s="12">
         <v>2021</v>
       </c>
@@ -3522,15 +4381,18 @@
         <v>71</v>
       </c>
       <c r="E79" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>71.153959079980268</v>
       </c>
       <c r="F79" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-0.15395907998026814</v>
       </c>
-    </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G79" s="31"/>
+      <c r="H79" s="31"/>
+      <c r="I79" s="31"/>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C80" s="12">
         <v>2021.25</v>
       </c>
@@ -3538,17 +4400,170 @@
         <v>71</v>
       </c>
       <c r="E80" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>71.337164367490914</v>
       </c>
       <c r="F80" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-0.33716436749091372</v>
       </c>
+      <c r="G80" s="31"/>
+      <c r="H80" s="31"/>
+      <c r="I80" s="31"/>
+    </row>
+    <row r="81" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G81" s="32"/>
+      <c r="H81" s="32"/>
+      <c r="I81" s="32"/>
+    </row>
+    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G82" s="32"/>
+      <c r="H82" s="32"/>
+      <c r="I82" s="32"/>
+    </row>
+    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G83" s="32"/>
+      <c r="H83" s="32"/>
+      <c r="I83" s="32"/>
+    </row>
+    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="32"/>
+    </row>
+    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G85" s="32"/>
+      <c r="H85" s="32"/>
+      <c r="I85" s="32"/>
+    </row>
+    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G86" s="32"/>
+      <c r="H86" s="32"/>
+      <c r="I86" s="32"/>
+    </row>
+    <row r="87" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G87" s="32"/>
+      <c r="H87" s="32"/>
+      <c r="I87" s="32"/>
+    </row>
+    <row r="88" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G88" s="32"/>
+      <c r="H88" s="32"/>
+      <c r="I88" s="32"/>
+    </row>
+    <row r="89" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G89" s="32"/>
+      <c r="H89" s="32"/>
+      <c r="I89" s="32"/>
+    </row>
+    <row r="90" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G90" s="32"/>
+      <c r="H90" s="32"/>
+      <c r="I90" s="32"/>
+    </row>
+    <row r="91" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G91" s="32"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="32"/>
+    </row>
+    <row r="92" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G92" s="32"/>
+      <c r="H92" s="32"/>
+      <c r="I92" s="32"/>
+    </row>
+    <row r="93" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G93" s="32"/>
+      <c r="H93" s="32"/>
+      <c r="I93" s="32"/>
+    </row>
+    <row r="94" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="32"/>
+    </row>
+    <row r="95" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G95" s="32"/>
+      <c r="H95" s="32"/>
+      <c r="I95" s="32"/>
+    </row>
+    <row r="96" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G96" s="32"/>
+      <c r="H96" s="32"/>
+      <c r="I96" s="32"/>
+    </row>
+    <row r="97" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G97" s="32"/>
+      <c r="H97" s="32"/>
+      <c r="I97" s="32"/>
+    </row>
+    <row r="98" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
+      <c r="I98" s="32"/>
+    </row>
+    <row r="99" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G99" s="32"/>
+      <c r="H99" s="32"/>
+      <c r="I99" s="32"/>
+    </row>
+    <row r="100" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G100" s="32"/>
+      <c r="H100" s="32"/>
+      <c r="I100" s="32"/>
+    </row>
+    <row r="101" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G101" s="32"/>
+      <c r="H101" s="32"/>
+      <c r="I101" s="32"/>
+    </row>
+    <row r="102" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G102" s="32"/>
+      <c r="H102" s="32"/>
+      <c r="I102" s="32"/>
+    </row>
+    <row r="103" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G103" s="32"/>
+      <c r="H103" s="32"/>
+      <c r="I103" s="32"/>
+    </row>
+    <row r="104" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G104" s="32"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="32"/>
+    </row>
+    <row r="105" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G105" s="32"/>
+      <c r="H105" s="32"/>
+      <c r="I105" s="32"/>
+    </row>
+    <row r="106" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G106" s="32"/>
+      <c r="H106" s="32"/>
+      <c r="I106" s="32"/>
+    </row>
+    <row r="107" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G107" s="32"/>
+      <c r="H107" s="32"/>
+      <c r="I107" s="32"/>
+    </row>
+    <row r="108" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G108" s="32"/>
+      <c r="H108" s="32"/>
+      <c r="I108" s="32"/>
+    </row>
+    <row r="109" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G109" s="32"/>
+      <c r="H109" s="32"/>
+      <c r="I109" s="32"/>
+    </row>
+    <row r="110" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G110" s="32"/>
+      <c r="H110" s="32"/>
+      <c r="I110" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="K11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>